<commit_message>
update with heatmap, commine line options and hippo fns
</commit_message>
<xml_diff>
--- a/misc/marker_genes.xlsx
+++ b/misc/marker_genes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanli/Desktop/scRIC_development/scRICA/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E2F0EF-1358-0047-8468-4756A2B255F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CADD42-F907-6A44-9A7D-48A74FCA6974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24120" windowHeight="17800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7600" yWindow="4220" windowWidth="24120" windowHeight="17800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fallopian Tube Markers" sheetId="1" r:id="rId1"/>
@@ -273,7 +273,7 @@
     <t>ALDH3B2</t>
   </si>
   <si>
-    <t>cellType</t>
+    <t>geneType</t>
   </si>
 </sst>
 </file>

</xml_diff>